<commit_message>
Full unfolded order list, start of gantt
</commit_message>
<xml_diff>
--- a/input/input.xlsx
+++ b/input/input.xlsx
@@ -181,7 +181,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="#,##0%"/>
   </numFmts>
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -194,6 +194,12 @@
       <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
       <family val="2"/>
     </font>
     <font>
@@ -244,67 +250,67 @@
     <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="3" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf xfId="0" numFmtId="4" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="3" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf xfId="0" numFmtId="4" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="3" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+      <alignment horizontal="general"/>
+    </xf>
+    <xf xfId="0" numFmtId="4" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="4" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf xfId="0" numFmtId="4" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="general"/>
     </xf>
     <xf xfId="0" numFmtId="4" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="general"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="3" applyFont="1" fillId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="general"/>
-    </xf>
-    <xf xfId="0" numFmtId="4" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="general"/>
-    </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="general"/>
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf xfId="0" numFmtId="164" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="4" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf xfId="0" numFmtId="164" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="3" applyFont="1" fillId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf xfId="0" numFmtId="164" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">

</xml_diff>